<commit_message>
Modify prc;xlsx verify link with app
</commit_message>
<xml_diff>
--- a/prc.xlsx
+++ b/prc.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">**Accessible**</t>
   </si>
   <si>
-    <t xml:space="preserve">  accessibility  by  supporting  not  only  the  accessibility  of  the  text  content  of  a  document,  but  also  the  accessibility  of  the  text  signals. -------------------------------------------------------  The  accessibility  of  documents  can  be  analyzed  in  the  following  four  dimensions:  technological (line.2),  legal (line.4),  economic (line.5) and social/ethical(line.3). </t>
+    <t xml:space="preserve"> Accessibility  by  supporting  not  only  the  accessibility  of  the  text  content  of  a  document,  but  also  the  accessibility  of  the  text  signals. -------------------------------------------------------  The  accessibility  of  documents  can  be  analyzed  in  the  following  four  dimensions:  technological (line.2),  legal (line.4),  economic (line.5) and social/ethical(line.3). </t>
   </si>
   <si>
     <t xml:space="preserve">**Accessible au plus grand nombre**</t>
@@ -946,10 +946,10 @@
   <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.15"/>
@@ -2005,7 +2005,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>

</xml_diff>

<commit_message>
git import apps 0.3
</commit_message>
<xml_diff>
--- a/prc.xlsx
+++ b/prc.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">**Accessible**</t>
   </si>
   <si>
-    <t xml:space="preserve"> Accessibility  by  supporting  not  only  the  accessibility  of  the  text  content  of  a  document,  but  also  the  accessibility  of  the  text  signals. -------------------------------------------------------  The  accessibility  of  documents  can  be  analyzed  in  the  following  four  dimensions:  technological (line.2),  legal (line.4),  economic (line.5) and social/ethical(line.3). </t>
+    <t xml:space="preserve"> accessibility  by  supporting  not  only              the  content text  accessibility  of  a  document,  but  also  the  accessibility  of  the  text  signals. -------------------------------------------------------  The  accessibility  of  documents  can  be  analyzed  in  the  following  four  dimensions:  technological (line.2),  legal (line.4),  economic (line.5) and social/ethical(line.3). </t>
   </si>
   <si>
     <t xml:space="preserve">**Accessible au plus grand nombre**</t>
@@ -949,7 +949,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="77.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.15"/>
@@ -2005,7 +2005,7 @@
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>

</xml_diff>